<commit_message>
#275493 2 more cases done - 2 left
</commit_message>
<xml_diff>
--- a/PlaywrightTests/CMB/QA/Catalog_scf_XLSX_u.xlsx
+++ b/PlaywrightTests/CMB/QA/Catalog_scf_XLSX_u.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\RegoMarketplace\smoke-auto-cm\PlaywrightTests\CMB\QA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B793C548-7065-4A9B-9EF8-2E6A866B4969}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0765F97D-5AE2-4936-9ED7-933290622E7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8235" yWindow="9585" windowWidth="20985" windowHeight="9705" tabRatio="818" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13605" yWindow="855" windowWidth="20985" windowHeight="9705" tabRatio="818" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Header" sheetId="3" r:id="rId1"/>
@@ -2297,11 +2297,12 @@
   <dimension ref="A1:DW12"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
+    <col min="1" max="1" width="22.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.5703125" customWidth="1"/>
     <col min="4" max="4" width="25.85546875" customWidth="1"/>
     <col min="6" max="6" width="27.42578125" customWidth="1"/>

</xml_diff>